<commit_message>
modified design project, added searchShopByKeyword() in ShopService and implement in ShopServiceIpm, added API /searchShopByKeyword/{product}, added findByNameContainingIgnoreCase(String keyword) in ShopRepo, fix ten -> name in entity Shop
</commit_message>
<xml_diff>
--- a/design_profject/project.xlsx
+++ b/design_profject/project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NGUYEN THANH NAM\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6459EA06-E66E-45BB-B29C-5E2E6D4697E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E495D42C-723F-4456-B467-F9E5D4F815CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>Thiết kế phần mềm quản lí cửa hàng</t>
   </si>
@@ -261,21 +261,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">   phẩm, tính toán số lượng sản phẩm đã bán, còn lại trong cửa hàng,tính value theo số lượng, hoàn thiện api cho tính năng </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(6 ngày)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">hoàn thiện api tính năng </t>
     </r>
     <r>
@@ -329,39 +314,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">2, shop-feature : tạo ShopService, thêm, sửa, xóa, cập nhật, tìm kiếm, lấy thông tin 1 hoặc nhiều phiếu nhập và xuất sản phẩm, kiểm tra số lượng tồn kho,  hoàn thiện api tính năng </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(5 ngày)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">3, product-feature : tạo ProductService, code các tính năng thêm, cập nhật, xóa, tìm kiếm, lấy thông tin 1 hoặc nhiều sản </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">4, user-feature : tạo UserService thêm, sửa, xóa, tìm kiếm, lấy thông 1 hoặc nhiều user, hoàn thiện api tính năng </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(5 ngày)</t>
-    </r>
-  </si>
-  <si>
     <t>1, Quản lí shop :   thêm, sửa, xóa, tìm kiếm, lấy thông 1 hoặc nhiều cửa hàng</t>
   </si>
   <si>
@@ -384,57 +336,6 @@
   </si>
   <si>
     <t>4, Quản lí  nhân account : thêm, sửa, xóa, tìm kiếm, lấy thông 1 hoặc nhiều account, cấp tài khoản cho user</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">7, order-feature : tạo OrderService, thêm, sửa, xóa, cập nhật, tìm kiếm, lấy thông tin 1 hoặc nhiều đơn hàng, hoàn thiện api tính năng </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(5 ngày)</t>
-    </r>
-  </si>
-  <si>
-    <t>8, statistical-feature : tạo StatisticalService, thống kê 2 bảng  : bảng statistical product thống kê (sản phẩm trong kho, trong cửa hàng, đã bán và hạn sử dụng)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9, security-feature : </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">5, account-feature : tạo AccountService, thêm, sửa, xóa, tìm kiếm, lấy thông 1 hoặc nhiều account, hoàn thiện api tính năng </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(3ngày)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>6, role-feature : tạo RoleService, thêm, sửa, xóa, tìm kiếm, lấy thông 1 hoặc nhiều role, hoàn thiện api tính năng</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(2 ngày)</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">                 bảng revenue-profit thống kê (tên sản phẩm, số lượng bán, doanh thu, lợi nhuận theo ngày, tháng)</t>
@@ -456,7 +357,91 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">10, exception-feature : tao 1 class Exception để bắt các lỗi trong complie time </t>
+      <t xml:space="preserve">2, shop-feature : tạo ShopService, thêm, sửa, xóa, cập nhật, tìm kiếm, lấy thông tin 1 hoặc nhiều shop,  hoàn thiện api tính năng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1 ngày)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3, user-feature : tạo UserService thêm, sửa, xóa, tìm kiếm, lấy thông 1 hoặc nhiều user, hoàn thiện api tính năng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(5 ngày)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4, account-feature : tạo AccountService, thêm, sửa, xóa, tìm kiếm, lấy thông 1 hoặc nhiều account, hoàn thiện api tính năng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(3ngày)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">7, product-feature : tạo ProductService, code các tính năng thêm, cập nhật, xóa, tìm kiếm, lấy thông tin 1 hoặc nhiều sản </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8, order-feature : tạo OrderService, thêm, sửa, xóa, cập nhật, tìm kiếm, lấy thông tin 1 hoặc nhiều đơn hàng, hoàn thiện api tính năng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(5 ngày)</t>
+    </r>
+  </si>
+  <si>
+    <t>9, statistical-feature : tạo StatisticalService, thống kê 2 bảng  : bảng statistical product thống kê (sản phẩm trong kho, trong cửa hàng, đã bán và hạn sử dụng)</t>
+  </si>
+  <si>
+    <r>
+      <t>5, role-feature : tạo RoleService, thêm, sửa, xóa, tìm kiếm, lấy thông 1 hoặc nhiều role, hoàn thiện api tính năng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2 ngày)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">10, security-feature : </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">11, exception-feature : tao 1 class Exception để bắt các lỗi trong complie time </t>
     </r>
     <r>
       <rPr>
@@ -467,6 +452,42 @@
         <scheme val="minor"/>
       </rPr>
       <t>(4 ngày)</t>
+    </r>
+  </si>
+  <si>
+    <t>6 store-shop-feature :  tạo StoreShopService, thêm, sửa, xóa, cập nhật, tìm kiếm, lấy thông tin 1 hoặc nhiều phiếu nhập và xuất sản phẩm, kiểm tra số lượng tồn kho,</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  hoàn thiện api tính năng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(4 ngày)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">phẩm, tính toán số lượng sản phẩm đã bán, còn lại trong cửa hàng,tính value theo số lượng, hoàn thiện api cho tính năng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(6 ngày)</t>
     </r>
   </si>
 </sst>
@@ -623,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -672,11 +693,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2909,10 +2926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE139"/>
+  <dimension ref="A1:AE141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="M111" sqref="M111"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="N90" sqref="N90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3866,33 +3883,33 @@
     </row>
     <row r="69" spans="1:24" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A69" s="10"/>
-      <c r="B69" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="28"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28"/>
-      <c r="K69" s="28"/>
-      <c r="L69" s="28"/>
-      <c r="M69" s="28"/>
-      <c r="N69" s="28"/>
-      <c r="O69" s="28"/>
-      <c r="P69" s="28"/>
-      <c r="Q69" s="28"/>
-      <c r="R69" s="28"/>
-      <c r="S69" s="28"/>
-      <c r="T69" s="28"/>
-      <c r="U69" s="28"/>
+      <c r="B69" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="11"/>
+      <c r="L69" s="11"/>
+      <c r="M69" s="11"/>
+      <c r="N69" s="11"/>
+      <c r="O69" s="11"/>
+      <c r="P69" s="11"/>
+      <c r="Q69" s="11"/>
+      <c r="R69" s="11"/>
+      <c r="S69" s="11"/>
+      <c r="T69" s="11"/>
+      <c r="U69" s="11"/>
     </row>
     <row r="70" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A70" s="5"/>
       <c r="B70" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -3920,7 +3937,7 @@
     <row r="71" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -3942,7 +3959,7 @@
     <row r="72" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A72" s="5"/>
       <c r="B72" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -3966,7 +3983,7 @@
     <row r="73" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A73" s="5"/>
       <c r="B73" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -3990,7 +4007,7 @@
     <row r="74" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -4012,7 +4029,7 @@
     <row r="75" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A75" s="5"/>
       <c r="B75" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -4038,7 +4055,7 @@
     <row r="76" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A76" s="5"/>
       <c r="B76" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -4127,7 +4144,7 @@
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
     </row>
-    <row r="81" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
       <c r="C81" s="1" t="s">
@@ -4142,7 +4159,7 @@
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
     </row>
-    <row r="82" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="1" t="s">
@@ -4157,7 +4174,7 @@
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
     </row>
-    <row r="83" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
       <c r="C83" s="1" t="s">
@@ -4172,7 +4189,7 @@
       <c r="J83" s="5"/>
       <c r="K83" s="5"/>
     </row>
-    <row r="84" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A84" s="5"/>
       <c r="B84" s="1" t="s">
         <v>33</v>
@@ -4187,7 +4204,7 @@
       <c r="J84" s="5"/>
       <c r="K84" s="5"/>
     </row>
-    <row r="85" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="1" t="s">
@@ -4202,7 +4219,7 @@
       <c r="J85" s="5"/>
       <c r="K85" s="5"/>
     </row>
-    <row r="86" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A86" s="5"/>
       <c r="B86" s="5"/>
       <c r="C86" s="1" t="s">
@@ -4217,7 +4234,7 @@
       <c r="J86" s="5"/>
       <c r="K86" s="5"/>
     </row>
-    <row r="87" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A87" s="5"/>
       <c r="B87" s="1" t="s">
         <v>36</v>
@@ -4232,7 +4249,7 @@
       <c r="J87" s="5"/>
       <c r="K87" s="5"/>
     </row>
-    <row r="88" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
@@ -4245,7 +4262,7 @@
       <c r="J88" s="5"/>
       <c r="K88" s="5"/>
     </row>
-    <row r="89" spans="1:30" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:23" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A89" s="9" t="s">
         <v>39</v>
       </c>
@@ -4260,7 +4277,7 @@
       <c r="J89" s="5"/>
       <c r="K89" s="5"/>
     </row>
-    <row r="90" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>45</v>
       </c>
@@ -4279,7 +4296,7 @@
       <c r="N90" s="5"/>
       <c r="O90" s="5"/>
     </row>
-    <row r="91" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A91" s="5"/>
       <c r="B91" s="5" t="s">
         <v>55</v>
@@ -4294,33 +4311,33 @@
       <c r="J91" s="5"/>
       <c r="K91" s="5"/>
     </row>
-    <row r="92" spans="1:30" ht="18" x14ac:dyDescent="0.35">
-      <c r="B92" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="27"/>
-      <c r="G92" s="27"/>
-      <c r="H92" s="27"/>
-      <c r="I92" s="27"/>
-      <c r="J92" s="27"/>
-      <c r="K92" s="27"/>
-      <c r="L92" s="27"/>
-      <c r="M92" s="27"/>
-      <c r="N92" s="27"/>
-      <c r="O92" s="27"/>
-      <c r="P92" s="27"/>
-      <c r="Q92" s="27"/>
-      <c r="R92" s="27"/>
-      <c r="S92" s="27"/>
-      <c r="T92" s="27"/>
-      <c r="U92" s="27"/>
-    </row>
-    <row r="93" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="B92" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
+      <c r="I92" s="5"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="5"/>
+      <c r="L92" s="5"/>
+      <c r="M92" s="5"/>
+      <c r="N92" s="5"/>
+      <c r="O92" s="5"/>
+      <c r="P92" s="5"/>
+      <c r="Q92" s="5"/>
+      <c r="R92" s="5"/>
+      <c r="S92" s="5"/>
+      <c r="T92" s="5"/>
+      <c r="U92" s="5"/>
+    </row>
+    <row r="93" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="B93" s="26" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C93" s="26"/>
       <c r="D93" s="26"/>
@@ -4344,42 +4361,35 @@
       <c r="V93" s="26"/>
       <c r="W93" s="26"/>
     </row>
-    <row r="94" spans="1:30" ht="18" x14ac:dyDescent="0.35">
-      <c r="B94" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C94" s="27"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="27"/>
-      <c r="F94" s="27"/>
-      <c r="G94" s="27"/>
-      <c r="H94" s="27"/>
-      <c r="I94" s="27"/>
-      <c r="J94" s="27"/>
-      <c r="K94" s="27"/>
-      <c r="L94" s="27"/>
-      <c r="M94" s="27"/>
-      <c r="N94" s="27"/>
-      <c r="O94" s="27"/>
-      <c r="P94" s="27"/>
-      <c r="Q94" s="27"/>
-      <c r="R94" s="5"/>
-      <c r="S94" s="5"/>
-      <c r="T94" s="5"/>
-      <c r="U94" s="5"/>
-      <c r="V94" s="5"/>
-      <c r="W94" s="5"/>
-      <c r="X94" s="5"/>
-      <c r="Y94" s="5"/>
-      <c r="Z94" s="5"/>
-      <c r="AA94" s="5"/>
-      <c r="AB94" s="5"/>
-      <c r="AC94" s="5"/>
-      <c r="AD94" s="5"/>
-    </row>
-    <row r="95" spans="1:30" ht="18" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="B94" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C94" s="26"/>
+      <c r="D94" s="26"/>
+      <c r="E94" s="26"/>
+      <c r="F94" s="26"/>
+      <c r="G94" s="26"/>
+      <c r="H94" s="26"/>
+      <c r="I94" s="26"/>
+      <c r="J94" s="26"/>
+      <c r="K94" s="26"/>
+      <c r="L94" s="26"/>
+      <c r="M94" s="26"/>
+      <c r="N94" s="26"/>
+      <c r="O94" s="26"/>
+      <c r="P94" s="26"/>
+      <c r="Q94" s="26"/>
+      <c r="R94" s="26"/>
+      <c r="S94" s="26"/>
+      <c r="T94" s="26"/>
+      <c r="U94" s="26"/>
+      <c r="V94" s="26"/>
+      <c r="W94" s="26"/>
+    </row>
+    <row r="95" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="B95" s="26" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="C95" s="26"/>
       <c r="D95" s="26"/>
@@ -4396,203 +4406,215 @@
       <c r="O95" s="26"/>
       <c r="P95" s="26"/>
       <c r="Q95" s="26"/>
-      <c r="R95" s="5"/>
-      <c r="S95" s="5"/>
-      <c r="T95" s="5"/>
-      <c r="U95" s="5"/>
-      <c r="V95" s="5"/>
-      <c r="W95" s="5"/>
-    </row>
-    <row r="96" spans="1:30" ht="18" x14ac:dyDescent="0.35">
-      <c r="B96" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="C96" s="27"/>
-      <c r="D96" s="27"/>
-      <c r="E96" s="27"/>
-      <c r="F96" s="27"/>
-      <c r="G96" s="27"/>
-      <c r="H96" s="27"/>
-      <c r="I96" s="27"/>
-      <c r="J96" s="27"/>
-      <c r="K96" s="27"/>
-      <c r="L96" s="27"/>
-      <c r="M96" s="27"/>
-      <c r="N96" s="27"/>
-      <c r="O96" s="27"/>
-      <c r="P96" s="27"/>
-      <c r="Q96" s="27"/>
-      <c r="R96" s="27"/>
-      <c r="S96" s="5"/>
-      <c r="T96" s="5"/>
-      <c r="U96" s="5"/>
-      <c r="V96" s="5"/>
-      <c r="W96" s="5"/>
-    </row>
-    <row r="97" spans="2:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B97" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C97" s="27"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="27"/>
-      <c r="H97" s="27"/>
-      <c r="I97" s="27"/>
-      <c r="J97" s="27"/>
-      <c r="K97" s="27"/>
-      <c r="L97" s="27"/>
-      <c r="M97" s="27"/>
-      <c r="N97" s="27"/>
-      <c r="O97" s="27"/>
-      <c r="P97" s="27"/>
-      <c r="Q97" s="27"/>
-      <c r="R97" s="27"/>
-      <c r="S97" s="27"/>
-      <c r="T97" s="27"/>
-      <c r="U97" s="5"/>
-      <c r="V97" s="5"/>
-      <c r="W97" s="5"/>
-    </row>
-    <row r="98" spans="2:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B98" s="27" t="s">
+      <c r="R95" s="26"/>
+      <c r="S95" s="26"/>
+      <c r="T95" s="26"/>
+      <c r="U95" s="26"/>
+      <c r="V95" s="26"/>
+      <c r="W95" s="26"/>
+    </row>
+    <row r="96" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="B96" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="27"/>
-      <c r="H98" s="27"/>
-      <c r="I98" s="27"/>
-      <c r="J98" s="27"/>
-      <c r="K98" s="27"/>
-      <c r="L98" s="27"/>
-      <c r="M98" s="27"/>
-      <c r="N98" s="27"/>
-      <c r="O98" s="27"/>
-      <c r="P98" s="27"/>
-      <c r="Q98" s="27"/>
-      <c r="R98" s="27"/>
-      <c r="S98" s="27"/>
-      <c r="T98" s="27"/>
-      <c r="U98" s="27"/>
-      <c r="V98" s="5"/>
-      <c r="W98" s="5"/>
-    </row>
-    <row r="99" spans="2:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B99" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="C99" s="27"/>
-      <c r="D99" s="27"/>
-      <c r="E99" s="27"/>
-      <c r="F99" s="27"/>
-      <c r="G99" s="27"/>
-      <c r="H99" s="27"/>
-      <c r="I99" s="27"/>
-      <c r="J99" s="27"/>
-      <c r="K99" s="27"/>
-      <c r="L99" s="27"/>
-      <c r="M99" s="27"/>
-      <c r="N99" s="27"/>
-      <c r="O99" s="27"/>
-      <c r="P99" s="27"/>
-      <c r="Q99" s="27"/>
-      <c r="R99" s="27"/>
-      <c r="S99" s="27"/>
-      <c r="T99" s="27"/>
-      <c r="U99" s="5"/>
-      <c r="V99" s="5"/>
+      <c r="C96" s="26"/>
+      <c r="D96" s="26"/>
+      <c r="E96" s="26"/>
+      <c r="F96" s="26"/>
+      <c r="G96" s="26"/>
+      <c r="H96" s="26"/>
+      <c r="I96" s="26"/>
+      <c r="J96" s="26"/>
+      <c r="K96" s="26"/>
+      <c r="L96" s="26"/>
+      <c r="M96" s="26"/>
+      <c r="N96" s="26"/>
+      <c r="O96" s="26"/>
+      <c r="P96" s="26"/>
+      <c r="Q96" s="26"/>
+      <c r="R96" s="26"/>
+      <c r="S96" s="26"/>
+      <c r="T96" s="26"/>
+      <c r="U96" s="26"/>
+      <c r="V96" s="26"/>
+      <c r="W96" s="26"/>
+    </row>
+    <row r="97" spans="2:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="B97" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C97" s="26"/>
+      <c r="D97" s="26"/>
+      <c r="E97" s="26"/>
+      <c r="F97" s="26"/>
+      <c r="G97" s="26"/>
+      <c r="H97" s="26"/>
+      <c r="I97" s="26"/>
+      <c r="J97" s="26"/>
+      <c r="K97" s="26"/>
+      <c r="L97" s="26"/>
+      <c r="M97" s="26"/>
+      <c r="N97" s="26"/>
+      <c r="O97" s="26"/>
+      <c r="P97" s="26"/>
+      <c r="Q97" s="26"/>
+      <c r="R97" s="26"/>
+      <c r="S97" s="26"/>
+      <c r="T97" s="26"/>
+      <c r="U97" s="26"/>
+      <c r="V97" s="26"/>
+      <c r="W97" s="26"/>
+      <c r="X97" s="26"/>
+    </row>
+    <row r="98" spans="2:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="B98" s="13"/>
+      <c r="C98" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D98" s="26"/>
+      <c r="E98" s="26"/>
+      <c r="F98" s="26"/>
+      <c r="G98" s="26"/>
+      <c r="H98" s="26"/>
+      <c r="I98" s="26"/>
+      <c r="J98" s="26"/>
+      <c r="K98" s="13"/>
+      <c r="L98" s="13"/>
+      <c r="M98" s="13"/>
+      <c r="N98" s="13"/>
+      <c r="O98" s="13"/>
+      <c r="P98" s="13"/>
+      <c r="Q98" s="13"/>
+      <c r="R98" s="13"/>
+      <c r="S98" s="13"/>
+      <c r="T98" s="13"/>
+      <c r="U98" s="13"/>
+      <c r="V98" s="13"/>
+      <c r="W98" s="13"/>
+      <c r="X98" s="26"/>
+    </row>
+    <row r="99" spans="2:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="B99" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C99" s="26"/>
+      <c r="D99" s="26"/>
+      <c r="E99" s="26"/>
+      <c r="F99" s="26"/>
+      <c r="G99" s="26"/>
+      <c r="H99" s="26"/>
+      <c r="I99" s="26"/>
+      <c r="J99" s="26"/>
+      <c r="K99" s="26"/>
+      <c r="L99" s="26"/>
+      <c r="M99" s="26"/>
+      <c r="N99" s="26"/>
+      <c r="O99" s="26"/>
+      <c r="P99" s="26"/>
+      <c r="Q99" s="26"/>
+      <c r="R99" s="26"/>
+      <c r="S99" s="26"/>
+      <c r="T99" s="26"/>
+      <c r="U99" s="26"/>
+      <c r="V99" s="26"/>
       <c r="W99" s="5"/>
-    </row>
-    <row r="100" spans="2:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B100" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
-      <c r="K100" s="1"/>
-      <c r="L100" s="1"/>
-      <c r="M100" s="1"/>
-      <c r="N100" s="1"/>
-      <c r="O100" s="1"/>
-      <c r="P100" s="1"/>
-      <c r="Q100" s="1"/>
-      <c r="R100" s="1"/>
-      <c r="S100" s="1"/>
-      <c r="T100" s="1"/>
+      <c r="X99" s="5"/>
+      <c r="Y99" s="5"/>
+      <c r="Z99" s="5"/>
+      <c r="AA99" s="5"/>
+      <c r="AB99" s="5"/>
+      <c r="AC99" s="5"/>
+      <c r="AD99" s="5"/>
+    </row>
+    <row r="100" spans="2:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="B100" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C100" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="D100" s="26"/>
+      <c r="E100" s="26"/>
+      <c r="F100" s="26"/>
+      <c r="G100" s="26"/>
+      <c r="H100" s="26"/>
+      <c r="I100" s="26"/>
+      <c r="J100" s="26"/>
+      <c r="K100" s="26"/>
+      <c r="L100" s="26"/>
+      <c r="M100" s="26"/>
+      <c r="N100" s="26"/>
+      <c r="O100" s="26"/>
+      <c r="P100" s="26"/>
+      <c r="Q100" s="26"/>
+      <c r="R100" s="5"/>
+      <c r="S100" s="5"/>
+      <c r="T100" s="5"/>
       <c r="U100" s="5"/>
       <c r="V100" s="5"/>
       <c r="W100" s="5"/>
     </row>
-    <row r="101" spans="2:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B101" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="C101" s="27"/>
-      <c r="D101" s="27"/>
-      <c r="E101" s="27"/>
-      <c r="F101" s="27"/>
-      <c r="G101" s="27"/>
-      <c r="H101" s="27"/>
-      <c r="I101" s="27"/>
-      <c r="J101" s="27"/>
-      <c r="K101" s="27"/>
-      <c r="L101" s="27"/>
-      <c r="M101" s="27"/>
-      <c r="N101" s="27"/>
-      <c r="O101" s="27"/>
-      <c r="P101" s="27"/>
-      <c r="Q101" s="27"/>
-      <c r="R101" s="27"/>
-      <c r="S101" s="27"/>
-      <c r="T101" s="27"/>
+    <row r="101" spans="2:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="B101" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C101" s="26"/>
+      <c r="D101" s="26"/>
+      <c r="E101" s="26"/>
+      <c r="F101" s="26"/>
+      <c r="G101" s="26"/>
+      <c r="H101" s="26"/>
+      <c r="I101" s="26"/>
+      <c r="J101" s="26"/>
+      <c r="K101" s="26"/>
+      <c r="L101" s="26"/>
+      <c r="M101" s="26"/>
+      <c r="N101" s="26"/>
+      <c r="O101" s="26"/>
+      <c r="P101" s="26"/>
+      <c r="Q101" s="26"/>
+      <c r="R101" s="26"/>
+      <c r="S101" s="5"/>
+      <c r="T101" s="5"/>
       <c r="U101" s="5"/>
       <c r="V101" s="5"/>
-    </row>
-    <row r="102" spans="2:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B102" s="5"/>
-      <c r="C102" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5"/>
-      <c r="H102" s="5"/>
-      <c r="I102" s="5"/>
-      <c r="J102" s="5"/>
-      <c r="K102" s="5"/>
-      <c r="L102" s="5"/>
-      <c r="M102" s="5"/>
-      <c r="N102" s="5"/>
-      <c r="O102" s="5"/>
-      <c r="P102" s="5"/>
-      <c r="Q102" s="5"/>
-      <c r="R102" s="5"/>
-      <c r="S102" s="5"/>
-      <c r="T102" s="5"/>
+      <c r="W101" s="5"/>
+    </row>
+    <row r="102" spans="2:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="B102" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="1"/>
+      <c r="S102" s="1"/>
+      <c r="T102" s="1"/>
       <c r="U102" s="5"/>
       <c r="V102" s="5"/>
       <c r="W102" s="5"/>
     </row>
-    <row r="103" spans="2:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B103" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C103" s="27"/>
-      <c r="D103" s="27"/>
-      <c r="E103" s="27"/>
-      <c r="F103" s="27"/>
-      <c r="G103" s="27"/>
+    <row r="103" spans="2:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="B103" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
       <c r="H103" s="5"/>
       <c r="I103" s="5"/>
       <c r="J103" s="5"/>
@@ -4608,12 +4630,11 @@
       <c r="T103" s="5"/>
       <c r="U103" s="5"/>
       <c r="V103" s="5"/>
-      <c r="W103" s="5"/>
-    </row>
-    <row r="104" spans="2:23" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="2:30" ht="18" x14ac:dyDescent="0.35">
       <c r="B104" s="5"/>
       <c r="C104" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D104" s="5"/>
       <c r="E104" s="5"/>
@@ -4636,11 +4657,11 @@
       <c r="V104" s="5"/>
       <c r="W104" s="5"/>
     </row>
-    <row r="105" spans="2:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B105" s="5"/>
-      <c r="C105" s="5" t="s">
-        <v>63</v>
-      </c>
+    <row r="105" spans="2:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="B105" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C105" s="5"/>
       <c r="D105" s="5"/>
       <c r="E105" s="5"/>
       <c r="F105" s="5"/>
@@ -4662,10 +4683,10 @@
       <c r="V105" s="5"/>
       <c r="W105" s="5"/>
     </row>
-    <row r="106" spans="2:23" ht="18" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:30" ht="18" x14ac:dyDescent="0.35">
       <c r="B106" s="5"/>
       <c r="C106" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D106" s="5"/>
       <c r="E106" s="5"/>
@@ -4688,10 +4709,10 @@
       <c r="V106" s="5"/>
       <c r="W106" s="5"/>
     </row>
-    <row r="107" spans="2:23" ht="18" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:30" ht="18" x14ac:dyDescent="0.35">
       <c r="B107" s="5"/>
       <c r="C107" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D107" s="5"/>
       <c r="E107" s="5"/>
@@ -4714,46 +4735,46 @@
       <c r="V107" s="5"/>
       <c r="W107" s="5"/>
     </row>
-    <row r="108" spans="2:23" ht="18" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:30" ht="18" x14ac:dyDescent="0.35">
       <c r="B108" s="5"/>
-      <c r="C108" s="15" t="s">
-        <v>68</v>
+      <c r="C108" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="D108" s="5"/>
       <c r="E108" s="5"/>
-      <c r="F108" s="13"/>
-      <c r="G108" s="13"/>
-      <c r="H108" s="13"/>
-      <c r="I108" s="13"/>
-      <c r="J108" s="13"/>
-      <c r="K108" s="13"/>
-      <c r="L108" s="13"/>
-      <c r="M108" s="13"/>
-      <c r="N108" s="13"/>
-      <c r="O108" s="13"/>
-      <c r="P108" s="13"/>
-      <c r="Q108" s="13"/>
-      <c r="R108" s="13"/>
-      <c r="S108" s="13"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="5"/>
+      <c r="I108" s="5"/>
+      <c r="J108" s="5"/>
+      <c r="K108" s="5"/>
+      <c r="L108" s="5"/>
+      <c r="M108" s="5"/>
+      <c r="N108" s="5"/>
+      <c r="O108" s="5"/>
+      <c r="P108" s="5"/>
+      <c r="Q108" s="5"/>
+      <c r="R108" s="5"/>
+      <c r="S108" s="5"/>
       <c r="T108" s="5"/>
       <c r="U108" s="5"/>
       <c r="V108" s="5"/>
       <c r="W108" s="5"/>
     </row>
-    <row r="109" spans="2:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B109" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="C109" s="27"/>
-      <c r="D109" s="27"/>
-      <c r="E109" s="27"/>
-      <c r="F109" s="27"/>
-      <c r="G109" s="27"/>
-      <c r="H109" s="27"/>
-      <c r="I109" s="27"/>
-      <c r="J109" s="27"/>
-      <c r="K109" s="27"/>
-      <c r="L109" s="27"/>
+    <row r="109" spans="2:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="B109" s="5"/>
+      <c r="C109" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5"/>
+      <c r="I109" s="5"/>
+      <c r="J109" s="5"/>
+      <c r="K109" s="5"/>
+      <c r="L109" s="5"/>
       <c r="M109" s="5"/>
       <c r="N109" s="5"/>
       <c r="O109" s="5"/>
@@ -4766,34 +4787,36 @@
       <c r="V109" s="5"/>
       <c r="W109" s="5"/>
     </row>
-    <row r="110" spans="2:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B110" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C110" s="15"/>
-      <c r="D110" s="15"/>
-      <c r="E110" s="15"/>
-      <c r="F110" s="5"/>
-      <c r="G110" s="5"/>
-      <c r="H110" s="5"/>
-      <c r="I110" s="5"/>
-      <c r="J110" s="5"/>
-      <c r="K110" s="5"/>
-      <c r="L110" s="5"/>
-      <c r="M110" s="5"/>
-      <c r="N110" s="5"/>
-      <c r="O110" s="5"/>
-      <c r="P110" s="5"/>
-      <c r="Q110" s="5"/>
-      <c r="R110" s="5"/>
-      <c r="S110" s="5"/>
+    <row r="110" spans="2:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="B110" s="5"/>
+      <c r="C110" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="13"/>
+      <c r="G110" s="13"/>
+      <c r="H110" s="13"/>
+      <c r="I110" s="13"/>
+      <c r="J110" s="13"/>
+      <c r="K110" s="13"/>
+      <c r="L110" s="13"/>
+      <c r="M110" s="13"/>
+      <c r="N110" s="13"/>
+      <c r="O110" s="13"/>
+      <c r="P110" s="13"/>
+      <c r="Q110" s="13"/>
+      <c r="R110" s="13"/>
+      <c r="S110" s="13"/>
       <c r="T110" s="5"/>
       <c r="U110" s="5"/>
       <c r="V110" s="5"/>
       <c r="W110" s="5"/>
     </row>
-    <row r="111" spans="2:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B111" s="5"/>
+    <row r="111" spans="2:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="B111" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
       <c r="E111" s="5"/>
@@ -4816,13 +4839,13 @@
       <c r="V111" s="5"/>
       <c r="W111" s="5"/>
     </row>
-    <row r="112" spans="2:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B112" s="5" t="s">
+    <row r="112" spans="2:30" ht="18" x14ac:dyDescent="0.35">
+      <c r="B112" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
+      <c r="C112" s="15"/>
+      <c r="D112" s="15"/>
+      <c r="E112" s="15"/>
       <c r="F112" s="5"/>
       <c r="G112" s="5"/>
       <c r="H112" s="5"/>
@@ -4843,9 +4866,7 @@
       <c r="W112" s="5"/>
     </row>
     <row r="113" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B113" s="5" t="s">
-        <v>72</v>
-      </c>
+      <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
       <c r="E113" s="5"/>
@@ -4869,7 +4890,9 @@
       <c r="W113" s="5"/>
     </row>
     <row r="114" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B114" s="5"/>
+      <c r="B114" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
       <c r="E114" s="5"/>
@@ -4892,26 +4915,25 @@
       <c r="V114" s="5"/>
       <c r="W114" s="5"/>
     </row>
-    <row r="115" spans="1:23" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A115" s="22" t="s">
+    <row r="115" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="B115" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B115" s="22"/>
-      <c r="C115" s="22"/>
-      <c r="D115" s="22"/>
-      <c r="E115" s="22"/>
-      <c r="F115" s="22"/>
-      <c r="G115" s="22"/>
-      <c r="H115" s="22"/>
-      <c r="I115" s="22"/>
-      <c r="J115" s="22"/>
-      <c r="K115" s="22"/>
-      <c r="L115" s="22"/>
-      <c r="M115" s="22"/>
-      <c r="N115" s="22"/>
-      <c r="O115" s="22"/>
-      <c r="P115" s="22"/>
-      <c r="Q115" s="22"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
+      <c r="I115" s="5"/>
+      <c r="J115" s="5"/>
+      <c r="K115" s="5"/>
+      <c r="L115" s="5"/>
+      <c r="M115" s="5"/>
+      <c r="N115" s="5"/>
+      <c r="O115" s="5"/>
+      <c r="P115" s="5"/>
+      <c r="Q115" s="5"/>
       <c r="R115" s="5"/>
       <c r="S115" s="5"/>
       <c r="T115" s="5"/>
@@ -4943,23 +4965,26 @@
       <c r="V116" s="5"/>
       <c r="W116" s="5"/>
     </row>
-    <row r="117" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="B117" s="5"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
-      <c r="G117" s="5"/>
-      <c r="H117" s="5"/>
-      <c r="I117" s="5"/>
-      <c r="J117" s="5"/>
-      <c r="K117" s="5"/>
-      <c r="L117" s="5"/>
-      <c r="M117" s="5"/>
-      <c r="N117" s="5"/>
-      <c r="O117" s="5"/>
-      <c r="P117" s="5"/>
-      <c r="Q117" s="5"/>
+    <row r="117" spans="1:23" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A117" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B117" s="22"/>
+      <c r="C117" s="22"/>
+      <c r="D117" s="22"/>
+      <c r="E117" s="22"/>
+      <c r="F117" s="22"/>
+      <c r="G117" s="22"/>
+      <c r="H117" s="22"/>
+      <c r="I117" s="22"/>
+      <c r="J117" s="22"/>
+      <c r="K117" s="22"/>
+      <c r="L117" s="22"/>
+      <c r="M117" s="22"/>
+      <c r="N117" s="22"/>
+      <c r="O117" s="22"/>
+      <c r="P117" s="22"/>
+      <c r="Q117" s="22"/>
       <c r="R117" s="5"/>
       <c r="S117" s="5"/>
       <c r="T117" s="5"/>
@@ -5495,12 +5520,58 @@
       <c r="V139" s="5"/>
       <c r="W139" s="5"/>
     </row>
+    <row r="140" spans="2:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="B140" s="5"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5"/>
+      <c r="E140" s="5"/>
+      <c r="F140" s="5"/>
+      <c r="G140" s="5"/>
+      <c r="H140" s="5"/>
+      <c r="I140" s="5"/>
+      <c r="J140" s="5"/>
+      <c r="K140" s="5"/>
+      <c r="L140" s="5"/>
+      <c r="M140" s="5"/>
+      <c r="N140" s="5"/>
+      <c r="O140" s="5"/>
+      <c r="P140" s="5"/>
+      <c r="Q140" s="5"/>
+      <c r="R140" s="5"/>
+      <c r="S140" s="5"/>
+      <c r="T140" s="5"/>
+      <c r="U140" s="5"/>
+      <c r="V140" s="5"/>
+      <c r="W140" s="5"/>
+    </row>
+    <row r="141" spans="2:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="B141" s="5"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="5"/>
+      <c r="E141" s="5"/>
+      <c r="F141" s="5"/>
+      <c r="G141" s="5"/>
+      <c r="H141" s="5"/>
+      <c r="I141" s="5"/>
+      <c r="J141" s="5"/>
+      <c r="K141" s="5"/>
+      <c r="L141" s="5"/>
+      <c r="M141" s="5"/>
+      <c r="N141" s="5"/>
+      <c r="O141" s="5"/>
+      <c r="P141" s="5"/>
+      <c r="Q141" s="5"/>
+      <c r="R141" s="5"/>
+      <c r="S141" s="5"/>
+      <c r="T141" s="5"/>
+      <c r="U141" s="5"/>
+      <c r="V141" s="5"/>
+      <c r="W141" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="O49:T50"/>
     <mergeCell ref="A1:P1"/>
-    <mergeCell ref="B93:W93"/>
-    <mergeCell ref="B95:Q95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>